<commit_message>
Concertado erro do arquivo
</commit_message>
<xml_diff>
--- a/webdev/materiais/tests/importacoes/entradas.xlsx
+++ b/webdev/materiais/tests/importacoes/entradas.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,6 +89,12 @@
       <b val="true"/>
       <sz val="11"/>
       <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -135,12 +141,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,17 +171,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -199,8 +209,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -222,12 +235,10 @@
       <c r="I2" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>